<commit_message>
Add elective assignment - Bipartite graph wasn't working for multiple edges so using multigraph   now - fixed bugs in cdc - added electives credits @Mathamind7 - added input file credits @AKASHMANDLA1438
Co-authored-by: Mathamind7 <parthn254@gmail.com>
Co-authored-by: AKASHMANDLA1438 <f20220807@goa.bits-pilani.ac.in>
</commit_message>
<xml_diff>
--- a/course_pref.xlsx
+++ b/course_pref.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saurav\Documents\sem3\Disco\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8DDC78-DD19-4FBE-BC94-8E0313B7BBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C715E6F-C7B1-49CD-8E52-3F596E56E631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{5C41911E-9A6B-496B-B5AE-CDCE0EE15155}"/>
   </bookViews>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="137">
   <si>
     <t>Professor</t>
   </si>
@@ -78,9 +69,6 @@
     <t>CS F429;CS F407;CS F413;CS F433;CS F441;CS F444;BITS F311;BITS F343;BITS F466;BITS F464;</t>
   </si>
   <si>
-    <t>CS F214;CS F111;CS F351;CS F213;CS F211;CS F303;CS F301;CS F342;CS F363;CS F364;</t>
-  </si>
-  <si>
     <t>CS G524;CS G513;</t>
   </si>
   <si>
@@ -102,18 +90,12 @@
     <t>BITS F311;CS F429;CS F433;CS F444;BITS F466;BITS F464;BITS F454;BITS F453;</t>
   </si>
   <si>
-    <t>CS F111;CS F222;CS F351;CS F213;CS F303;CS F214;CS F364;CS F212;CS F211;CS F301;</t>
-  </si>
-  <si>
     <t>CS G524;CS G513;CS G523;CS G526;CS G625;</t>
   </si>
   <si>
     <t>CS G513;CS G524;CS G525;CS G526;CS G623;</t>
   </si>
   <si>
-    <t>CSF 111;CSF 214;CS F222;CS F213;CS F215;CS F211;CS F241;CS F212;CS F351;CS F372;</t>
-  </si>
-  <si>
     <t>CS G523;CS G625;CS G526;</t>
   </si>
   <si>
@@ -141,9 +123,6 @@
     <t>CS F303;CS F301;CS F342;CS F363;CS F364;</t>
   </si>
   <si>
-    <t>CS F222;CS F215;CS F111;CS F303;CS F212;CS F213;CS F301;</t>
-  </si>
-  <si>
     <t>CS F213;CS F222;CS F111;CS F214;</t>
   </si>
   <si>
@@ -156,9 +135,6 @@
     <t>CS F301;CS F303;CS F364;CS F212;CS F215;CS F213;</t>
   </si>
   <si>
-    <t>CS F364;CS F215;CS F214;CS F222;CS F213;CS F212;CS F301;</t>
-  </si>
-  <si>
     <t>CS G523;CS G526;</t>
   </si>
   <si>
@@ -249,18 +225,9 @@
     <t>CS F303;CS F342;CS F364;CS F301;CS F363;</t>
   </si>
   <si>
-    <t>CS F215;CS F222;CS F214;CS F111;CS F301;CS F303;CS F342;CS F211;CS F212;</t>
-  </si>
-  <si>
     <t>CS F342;CS F363;CS F364;</t>
   </si>
   <si>
-    <t>CS F241;CS F372;CS F351;CS F372;CS F213;CS F214;CS F222;CS F215;</t>
-  </si>
-  <si>
-    <t>CS F351;CS F372;CS F215;CS F111;</t>
-  </si>
-  <si>
     <t>CS F213;CS F214;CS F215;</t>
   </si>
   <si>
@@ -355,6 +322,120 @@
   </si>
   <si>
     <t>CS G554;CS G527;</t>
+  </si>
+  <si>
+    <t>PROF-21</t>
+  </si>
+  <si>
+    <t>CS F212;CS F215;CS F301;CS F303;CS F342;CS F211;</t>
+  </si>
+  <si>
+    <t>CS F364;CS F215;CS F213;CS F212;</t>
+  </si>
+  <si>
+    <t>CS F222;CS F215;CS F111;CS F213;CS F301;</t>
+  </si>
+  <si>
+    <t>CS F111;CS F351;CS F213;CS F364;CS F211;</t>
+  </si>
+  <si>
+    <t>CS F214;CS F351;CS F213;CS F342;CS F363;CS F364;</t>
+  </si>
+  <si>
+    <t>CS F111;CS F213;CS F215;CS F241;CS F351;CS F372;</t>
+  </si>
+  <si>
+    <t>CS F364;CS F372;CS F212;</t>
+  </si>
+  <si>
+    <t>CS F433;BITS F386;CS F429;</t>
+  </si>
+  <si>
+    <t>CS G525;CS G524;</t>
+  </si>
+  <si>
+    <t>CS G516;CS G551;CS G553;CS G554;</t>
+  </si>
+  <si>
+    <t>PROF-22</t>
+  </si>
+  <si>
+    <t>PROF-23</t>
+  </si>
+  <si>
+    <t>PROF-24</t>
+  </si>
+  <si>
+    <t>PROF-25</t>
+  </si>
+  <si>
+    <t>PROF-26</t>
+  </si>
+  <si>
+    <t>PROF-27</t>
+  </si>
+  <si>
+    <t>PROF-28</t>
+  </si>
+  <si>
+    <t>PROF-29</t>
+  </si>
+  <si>
+    <t>PROF-30</t>
+  </si>
+  <si>
+    <t>CS F363;CS F342;</t>
+  </si>
+  <si>
+    <t>CS F372;CS F215;CS F111;</t>
+  </si>
+  <si>
+    <t>CS F241;CS F215;CS F213;</t>
+  </si>
+  <si>
+    <t>CS F211;CS F372;</t>
+  </si>
+  <si>
+    <t>CS F351;CS F372;CS F213;</t>
+  </si>
+  <si>
+    <t>CS F351;CS F363;CS F301;</t>
+  </si>
+  <si>
+    <t>CS F364;CS F303;CS F212;</t>
+  </si>
+  <si>
+    <t>CS F215;CS F211;CS F222;CS F213;</t>
+  </si>
+  <si>
+    <t>CS F342;CS F212;CS F303;</t>
+  </si>
+  <si>
+    <t>CS F222;CS F213;CS F363;CS F364;CS F211;</t>
+  </si>
+  <si>
+    <t>BITS F454;BITS F343;CS F441;CS F433;</t>
+  </si>
+  <si>
+    <t>BITS F452;BITS F364;BITS F464;</t>
+  </si>
+  <si>
+    <t>CS F413;CS F441;</t>
+  </si>
+  <si>
+    <t>BITS 466;CS F407;BITS F311;</t>
+  </si>
+  <si>
+    <t>BITS F386;BITS F312;</t>
+  </si>
+  <si>
+    <t>BITS F364;BITS F454;</t>
+  </si>
+  <si>
+    <t>BITS F386;BITS F452;BITS F453;</t>
+  </si>
+  <si>
+    <t>CS F407;CS F413;CS F441;CS F444;</t>
   </si>
 </sst>
 </file>
@@ -392,7 +473,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -575,6 +656,15 @@
         <color indexed="64"/>
       </left>
       <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -587,9 +677,6 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -631,7 +718,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -948,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D73C54D7-F43B-42DC-B2ED-2BD8C223B22C}">
-  <dimension ref="B1:G22"/>
+  <dimension ref="B1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -964,423 +1054,563 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="109.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="154.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="109.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="8" t="s">
+    <row r="5" spans="2:7" ht="115.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="101.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="8" t="s">
+      <c r="E7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="88.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G3" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="154.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="E8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="90.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="115.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="101.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="E9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="87.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="89.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="103.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="112.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="99" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="99" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="99.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="106.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="88.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="90.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="87.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="89.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="103.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="14" t="s">
+      <c r="F17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="97.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="97.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="114.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="112.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="99" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="99" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="G20" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="99" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F15" s="2" t="s">
+      <c r="F21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="112.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G15" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="99.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F16" s="2" t="s">
+      <c r="G22" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="106.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="97.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="97.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="114.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="99" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="112.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F22" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G22" s="17" t="s">
-        <v>18</v>
+      <c r="D23" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="96.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="102" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="112.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="103.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="105.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="105" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="99" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="G30" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="111" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="100.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>